<commit_message>
added some to README
</commit_message>
<xml_diff>
--- a/fakturor/Ikea.xlsx
+++ b/fakturor/Ikea.xlsx
@@ -996,7 +996,7 @@
         </is>
       </c>
       <c r="F9" s="42" t="n">
-        <v>169756</v>
+        <v>463399</v>
       </c>
       <c r="H9" s="5" t="n"/>
       <c r="I9" s="5" t="n"/>
@@ -1159,7 +1159,7 @@
         </is>
       </c>
       <c r="E15" s="12" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F15" s="12" t="inlineStr">
         <is>
@@ -1198,7 +1198,7 @@
         </is>
       </c>
       <c r="E16" s="21" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F16" s="22" t="n">
         <v>599</v>
@@ -1231,7 +1231,7 @@
         </is>
       </c>
       <c r="E17" s="23" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F17" s="24" t="n">
         <v>299</v>
@@ -1264,7 +1264,7 @@
         </is>
       </c>
       <c r="E18" s="21" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F18" s="22" t="n">
         <v>450</v>
@@ -1297,7 +1297,7 @@
         </is>
       </c>
       <c r="E19" s="23" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F19" s="24" t="n">
         <v>345</v>
@@ -1326,7 +1326,7 @@
       <c r="A20" s="10" t="n"/>
       <c r="B20" s="36" t="n"/>
       <c r="E20" s="21" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F20" s="22" t="n"/>
       <c r="G20" s="13" t="n"/>
@@ -1357,7 +1357,7 @@
         </is>
       </c>
       <c r="E21" s="21" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F21" s="25" t="n">
         <v>98</v>
@@ -1390,7 +1390,7 @@
         </is>
       </c>
       <c r="E22" s="23" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F22" s="27" t="n">
         <v>174</v>
@@ -1423,7 +1423,7 @@
         </is>
       </c>
       <c r="E23" s="21" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F23" s="25" t="n">
         <v>456</v>
@@ -1456,7 +1456,7 @@
         </is>
       </c>
       <c r="E24" s="23" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F24" s="27" t="n">
         <v>745</v>
@@ -1489,7 +1489,7 @@
         </is>
       </c>
       <c r="E25" s="21" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F25" s="25" t="n">
         <v>720</v>
@@ -1522,7 +1522,7 @@
         </is>
       </c>
       <c r="E26" s="23" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F26" s="27" t="n">
         <v>349</v>

</xml_diff>